<commit_message>
Add medical location case, add expected picture for firefox, change softassert to assert, remove unused page
</commit_message>
<xml_diff>
--- a/testdata/SearchAddress.xlsx
+++ b/testdata/SearchAddress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\GP\workspace3\OneMap\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AF2E9F-25A1-4BA7-9885-2A0B08D1532E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F5C9B4-93AD-4192-92FB-3EB6F6785131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>SearchAddress</t>
   </si>
   <si>
-    <t>BUKIT BATOK FLYOVER</t>
-  </si>
-  <si>
     <t>ASIAN CIVILISATIONS MUSEUM</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>UOB WEST MALL</t>
+  </si>
+  <si>
+    <t>BUKIT BATOK FIRE STATION</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,23 +394,23 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>